<commit_message>
add ring oscillator control, initial timing contraints
</commit_message>
<xml_diff>
--- a/doc/firmware-register-map-psec4a-evm.xlsx
+++ b/doc/firmware-register-map-psec4a-evm.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="52">
   <si>
     <t>Register Map</t>
   </si>
@@ -159,6 +159,27 @@
   </si>
   <si>
     <t>P-type transistor bias</t>
+  </si>
+  <si>
+    <t>LSB</t>
+  </si>
+  <si>
+    <t>ENABLE FIRMWARE FEEDBACK LOOP for ROvcp</t>
+  </si>
+  <si>
+    <t>ring oscillator counter divider output</t>
+  </si>
+  <si>
+    <t>trig sign - in psec4a serial block</t>
+  </si>
+  <si>
+    <t>dll speed select - in psec4a serial block</t>
+  </si>
+  <si>
+    <t>use reset in xfer process - in psec4a serial block</t>
+  </si>
+  <si>
+    <t>COUNT TARGET for ring osc when reg 0x52 enabled</t>
   </si>
 </sst>
 </file>
@@ -223,7 +244,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -271,14 +292,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -562,7 +584,7 @@
   <dimension ref="A1:G134"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="D107" sqref="D107"/>
+      <selection activeCell="C90" sqref="C90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -577,36 +599,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
+      <c r="B3" s="31"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
       <c r="F3" s="6"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="29"/>
-      <c r="B4" s="30"/>
+      <c r="A4" s="32"/>
+      <c r="B4" s="33"/>
       <c r="C4" s="1"/>
       <c r="D4" t="s">
         <v>15</v>
@@ -713,6 +735,9 @@
         <f t="shared" si="0"/>
         <v>x04</v>
       </c>
+      <c r="D11" s="28" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -723,7 +748,12 @@
         <f t="shared" si="0"/>
         <v>x05</v>
       </c>
-      <c r="D12" s="12"/>
+      <c r="C12" t="s">
+        <v>47</v>
+      </c>
+      <c r="D12" s="28" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
@@ -782,7 +812,7 @@
       <c r="C17" s="15"/>
       <c r="D17" s="15"/>
       <c r="E17" s="15"/>
-      <c r="F17" s="31"/>
+      <c r="F17" s="29"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="15">
@@ -796,7 +826,7 @@
       <c r="C18" s="15"/>
       <c r="D18" s="15"/>
       <c r="E18" s="15"/>
-      <c r="F18" s="32"/>
+      <c r="F18" s="30"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="15">
@@ -810,7 +840,7 @@
       <c r="C19" s="15"/>
       <c r="D19" s="15"/>
       <c r="E19" s="15"/>
-      <c r="F19" s="32"/>
+      <c r="F19" s="30"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="15">
@@ -824,7 +854,7 @@
       <c r="C20" s="15"/>
       <c r="D20" s="15"/>
       <c r="E20" s="15"/>
-      <c r="F20" s="32"/>
+      <c r="F20" s="30"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="15">
@@ -838,7 +868,7 @@
       <c r="C21" s="15"/>
       <c r="D21" s="15"/>
       <c r="E21" s="15"/>
-      <c r="F21" s="32"/>
+      <c r="F21" s="30"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="15">
@@ -852,7 +882,7 @@
       <c r="C22" s="15"/>
       <c r="D22" s="15"/>
       <c r="E22" s="15"/>
-      <c r="F22" s="32"/>
+      <c r="F22" s="30"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="15">
@@ -866,7 +896,7 @@
       <c r="C23" s="15"/>
       <c r="D23" s="15"/>
       <c r="E23" s="15"/>
-      <c r="F23" s="32"/>
+      <c r="F23" s="30"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="15">
@@ -880,7 +910,7 @@
       <c r="C24" s="15"/>
       <c r="D24" s="15"/>
       <c r="E24" s="15"/>
-      <c r="F24" s="32"/>
+      <c r="F24" s="30"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="15">
@@ -894,7 +924,7 @@
       <c r="C25" s="15"/>
       <c r="D25" s="15"/>
       <c r="E25" s="15"/>
-      <c r="F25" s="32"/>
+      <c r="F25" s="30"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="15">
@@ -908,7 +938,7 @@
       <c r="C26" s="15"/>
       <c r="D26" s="15"/>
       <c r="E26" s="15"/>
-      <c r="F26" s="32"/>
+      <c r="F26" s="30"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="15">
@@ -922,7 +952,7 @@
       <c r="C27" s="15"/>
       <c r="D27" s="15"/>
       <c r="E27" s="15"/>
-      <c r="F27" s="32"/>
+      <c r="F27" s="30"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="15">
@@ -936,7 +966,7 @@
       <c r="C28" s="15"/>
       <c r="D28" s="15"/>
       <c r="E28" s="15"/>
-      <c r="F28" s="32"/>
+      <c r="F28" s="30"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="15">
@@ -950,7 +980,7 @@
       <c r="C29" s="15"/>
       <c r="D29" s="15"/>
       <c r="E29" s="15"/>
-      <c r="F29" s="32"/>
+      <c r="F29" s="30"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="15">
@@ -964,7 +994,7 @@
       <c r="C30" s="15"/>
       <c r="D30" s="15"/>
       <c r="E30" s="15"/>
-      <c r="F30" s="32"/>
+      <c r="F30" s="30"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="15">
@@ -978,7 +1008,7 @@
       <c r="C31" s="15"/>
       <c r="D31" s="15"/>
       <c r="E31" s="15"/>
-      <c r="F31" s="32"/>
+      <c r="F31" s="30"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="15">
@@ -992,7 +1022,7 @@
       <c r="C32" s="15"/>
       <c r="D32" s="15"/>
       <c r="E32" s="15"/>
-      <c r="F32" s="32"/>
+      <c r="F32" s="30"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="15">
@@ -1006,7 +1036,7 @@
       <c r="C33" s="15"/>
       <c r="D33" s="15"/>
       <c r="E33" s="15"/>
-      <c r="F33" s="32"/>
+      <c r="F33" s="30"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="15">
@@ -1020,7 +1050,7 @@
       <c r="C34" s="15"/>
       <c r="D34" s="15"/>
       <c r="E34" s="15"/>
-      <c r="F34" s="32"/>
+      <c r="F34" s="30"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="15">
@@ -1034,7 +1064,7 @@
       <c r="C35" s="15"/>
       <c r="D35" s="15"/>
       <c r="E35" s="15"/>
-      <c r="F35" s="32"/>
+      <c r="F35" s="30"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="15">
@@ -1048,7 +1078,7 @@
       <c r="C36" s="15"/>
       <c r="D36" s="15"/>
       <c r="E36" s="15"/>
-      <c r="F36" s="32"/>
+      <c r="F36" s="30"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="15">
@@ -1062,7 +1092,7 @@
       <c r="C37" s="15"/>
       <c r="D37" s="15"/>
       <c r="E37" s="15"/>
-      <c r="F37" s="32"/>
+      <c r="F37" s="30"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="15">
@@ -1076,7 +1106,7 @@
       <c r="C38" s="15"/>
       <c r="D38" s="15"/>
       <c r="E38" s="15"/>
-      <c r="F38" s="32"/>
+      <c r="F38" s="30"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="15">
@@ -1090,7 +1120,7 @@
       <c r="C39" s="15"/>
       <c r="D39" s="15"/>
       <c r="E39" s="15"/>
-      <c r="F39" s="32"/>
+      <c r="F39" s="30"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="15">
@@ -1104,7 +1134,7 @@
       <c r="C40" s="15"/>
       <c r="D40" s="15"/>
       <c r="E40" s="15"/>
-      <c r="F40" s="32"/>
+      <c r="F40" s="30"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="15">
@@ -1118,7 +1148,7 @@
       <c r="C41" s="15"/>
       <c r="D41" s="15"/>
       <c r="E41" s="15"/>
-      <c r="F41" s="32"/>
+      <c r="F41" s="30"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42">
@@ -1645,7 +1675,9 @@
         <f t="shared" si="2"/>
         <v>x51</v>
       </c>
-      <c r="D88" s="5"/>
+      <c r="C88" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89">
@@ -1656,7 +1688,12 @@
         <f t="shared" si="2"/>
         <v>x52</v>
       </c>
-      <c r="D89" s="5"/>
+      <c r="C89" t="s">
+        <v>46</v>
+      </c>
+      <c r="D89" s="5" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90">
@@ -1667,7 +1704,12 @@
         <f t="shared" si="2"/>
         <v>x53</v>
       </c>
-      <c r="D90" s="5"/>
+      <c r="C90" t="s">
+        <v>48</v>
+      </c>
+      <c r="D90" s="5" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91">
@@ -1678,6 +1720,12 @@
         <f t="shared" si="2"/>
         <v>x54</v>
       </c>
+      <c r="C91" t="s">
+        <v>49</v>
+      </c>
+      <c r="D91" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92">
@@ -1688,7 +1736,12 @@
         <f t="shared" si="2"/>
         <v>x55</v>
       </c>
-      <c r="D92" s="5"/>
+      <c r="C92" t="s">
+        <v>50</v>
+      </c>
+      <c r="D92" t="s">
+        <v>45</v>
+      </c>
       <c r="E92" s="12"/>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
increase RO feedback counter to 32 bits
</commit_message>
<xml_diff>
--- a/doc/firmware-register-map-psec4a-evm.xlsx
+++ b/doc/firmware-register-map-psec4a-evm.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="54">
   <si>
     <t>Register Map</t>
   </si>
@@ -167,9 +167,6 @@
     <t>ENABLE FIRMWARE FEEDBACK LOOP for ROvcp</t>
   </si>
   <si>
-    <t>ring oscillator counter divider output</t>
-  </si>
-  <si>
     <t>trig sign - in psec4a serial block</t>
   </si>
   <si>
@@ -179,7 +176,16 @@
     <t>use reset in xfer process - in psec4a serial block</t>
   </si>
   <si>
-    <t>COUNT TARGET for ring osc when reg 0x52 enabled</t>
+    <t>ring oscillator counter divider output (low 16 bits)</t>
+  </si>
+  <si>
+    <t>ring oscillator counter divider output (high 16 bits)</t>
+  </si>
+  <si>
+    <t>COUNT TARGET (low 16 bits) for ring osc when reg 0x52 enabled</t>
+  </si>
+  <si>
+    <t>COUNT TARGET (high 16 bits) for ring osc when reg 0x52 enabled</t>
   </si>
 </sst>
 </file>
@@ -583,7 +589,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
       <selection activeCell="C90" sqref="C90"/>
     </sheetView>
   </sheetViews>
@@ -749,7 +755,7 @@
         <v>x05</v>
       </c>
       <c r="C12" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="D12" s="28" t="s">
         <v>9</v>
@@ -764,7 +770,12 @@
         <f t="shared" si="0"/>
         <v>x06</v>
       </c>
-      <c r="D13" s="12"/>
+      <c r="C13" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="D13" s="28" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
@@ -1665,6 +1676,9 @@
         <f t="shared" si="2"/>
         <v>x50</v>
       </c>
+      <c r="C87" s="28" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88">
@@ -1676,7 +1690,7 @@
         <v>x51</v>
       </c>
       <c r="C88" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
@@ -1705,7 +1719,7 @@
         <v>x53</v>
       </c>
       <c r="C90" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D90" s="5" t="s">
         <v>45</v>
@@ -1721,7 +1735,7 @@
         <v>x54</v>
       </c>
       <c r="C91" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D91" t="s">
         <v>45</v>
@@ -1737,7 +1751,7 @@
         <v>x55</v>
       </c>
       <c r="C92" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D92" t="s">
         <v>45</v>

</xml_diff>

<commit_message>
finished data handling, almost test ready
</commit_message>
<xml_diff>
--- a/doc/firmware-register-map-psec4a-evm.xlsx
+++ b/doc/firmware-register-map-psec4a-evm.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="66">
   <si>
     <t>Register Map</t>
   </si>
@@ -204,6 +204,24 @@
   </si>
   <si>
     <t>RO COUNT TARGET (high 16 bits) for ring osc when reg 0x52 enabled</t>
+  </si>
+  <si>
+    <t>readout: fifo select</t>
+  </si>
+  <si>
+    <t>value 1 to 8</t>
+  </si>
+  <si>
+    <t>adc start - delay between trigger and starting the ramp</t>
+  </si>
+  <si>
+    <t>readout: clk fifo readout</t>
+  </si>
+  <si>
+    <t>readout: reset fifo</t>
+  </si>
+  <si>
+    <t>data word</t>
   </si>
 </sst>
 </file>
@@ -268,7 +286,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -321,6 +339,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -612,8 +634,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C92" sqref="C92"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -628,38 +650,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="31"/>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
       <c r="F3" s="6"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="32"/>
-      <c r="B4" s="33"/>
+      <c r="A4" s="34"/>
+      <c r="B4" s="35"/>
       <c r="C4" s="1"/>
-      <c r="D4" s="34" t="s">
+      <c r="D4" s="36" t="s">
         <v>14</v>
       </c>
       <c r="F4" s="5" t="s">
@@ -670,7 +692,7 @@
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
-      <c r="D5" s="34"/>
+      <c r="D5" s="36"/>
     </row>
     <row r="6" spans="1:7" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
@@ -816,7 +838,9 @@
         <f t="shared" si="0"/>
         <v>x07</v>
       </c>
-      <c r="D15" s="11"/>
+      <c r="D15" s="31" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
@@ -827,7 +851,12 @@
         <f t="shared" si="0"/>
         <v>x08</v>
       </c>
-      <c r="D16" s="11"/>
+      <c r="C16" t="s">
+        <v>65</v>
+      </c>
+      <c r="D16" s="31" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
@@ -1614,8 +1643,12 @@
         <f t="shared" si="2"/>
         <v>x48</v>
       </c>
-      <c r="C80" s="8"/>
-      <c r="D80" s="8"/>
+      <c r="C80" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="D80" s="8" t="s">
+        <v>61</v>
+      </c>
       <c r="E80" s="8"/>
       <c r="F80" s="17"/>
     </row>
@@ -1686,6 +1719,9 @@
         <f t="shared" si="2"/>
         <v>x4E</v>
       </c>
+      <c r="C86" s="31" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87">
@@ -2332,6 +2368,9 @@
         <f t="shared" si="2"/>
         <v>x79</v>
       </c>
+      <c r="C129" s="31" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130">
@@ -2341,6 +2380,12 @@
       <c r="B130" s="19" t="str">
         <f t="shared" si="2"/>
         <v>x7A</v>
+      </c>
+      <c r="C130" t="s">
+        <v>63</v>
+      </c>
+      <c r="F130" s="32" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
prelim sine waves recorded, still need timing fixes in psec4a_core.vhd
</commit_message>
<xml_diff>
--- a/doc/firmware-register-map-psec4a-evm.xlsx
+++ b/doc/firmware-register-map-psec4a-evm.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="67">
   <si>
     <t>Register Map</t>
   </si>
@@ -222,6 +222,9 @@
   </si>
   <si>
     <t>data word</t>
+  </si>
+  <si>
+    <t>fifo used words</t>
   </si>
 </sst>
 </file>
@@ -634,8 +637,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -867,8 +870,12 @@
         <f t="shared" si="0"/>
         <v>x09</v>
       </c>
-      <c r="C17" s="5"/>
-      <c r="D17" s="11"/>
+      <c r="C17" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="D17" s="31" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="14">

</xml_diff>

<commit_message>
add bulk data readout
</commit_message>
<xml_diff>
--- a/doc/firmware-register-map-psec4a-evm.xlsx
+++ b/doc/firmware-register-map-psec4a-evm.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="73">
   <si>
     <t>Register Map</t>
   </si>
@@ -228,6 +228,21 @@
   </si>
   <si>
     <t>dll reset</t>
+  </si>
+  <si>
+    <t>readout: num usb words for register read</t>
+  </si>
+  <si>
+    <t>x000002</t>
+  </si>
+  <si>
+    <t>readout: num usb words for data read</t>
+  </si>
+  <si>
+    <t>x000422</t>
+  </si>
+  <si>
+    <t>readout: do a data read</t>
   </si>
 </sst>
 </file>
@@ -643,8 +658,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A118" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D136" sqref="D136"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C85" sqref="C85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1600,6 +1615,12 @@
         <f t="shared" si="2"/>
         <v>x44</v>
       </c>
+      <c r="C76" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="E76" s="12" t="s">
+        <v>69</v>
+      </c>
       <c r="F76" s="10"/>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
@@ -1611,8 +1632,13 @@
         <f t="shared" si="2"/>
         <v>x45</v>
       </c>
-      <c r="C77" s="8"/>
+      <c r="C77" s="12" t="s">
+        <v>70</v>
+      </c>
       <c r="D77" s="8"/>
+      <c r="E77" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="78" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="8">
@@ -1622,6 +1648,15 @@
       <c r="B78" s="19" t="str">
         <f t="shared" si="2"/>
         <v>x46</v>
+      </c>
+      <c r="C78" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="D78" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="E78" s="12" t="s">
+        <v>5</v>
       </c>
       <c r="F78" s="10"/>
     </row>

</xml_diff>

<commit_message>
add ping pong mode
</commit_message>
<xml_diff>
--- a/doc/firmware-register-map-psec4a-evm.xlsx
+++ b/doc/firmware-register-map-psec4a-evm.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="76">
   <si>
     <t>Register Map</t>
   </si>
@@ -243,6 +243,15 @@
   </si>
   <si>
     <t>external DAC vreset</t>
+  </si>
+  <si>
+    <t>psec4a_status_register</t>
+  </si>
+  <si>
+    <t>psec4a readout mode</t>
+  </si>
+  <si>
+    <t>0=all samples, 1=ping-pong 528-sample blocks</t>
   </si>
 </sst>
 </file>
@@ -307,7 +316,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -370,6 +379,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -658,8 +668,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C112" sqref="C112"/>
+    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D91" sqref="D91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -674,38 +684,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="34"/>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
+      <c r="B3" s="35"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
       <c r="F3" s="6"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="35"/>
-      <c r="B4" s="36"/>
+      <c r="A4" s="36"/>
+      <c r="B4" s="37"/>
       <c r="C4" s="1"/>
-      <c r="D4" s="37" t="s">
+      <c r="D4" s="38" t="s">
         <v>14</v>
       </c>
       <c r="F4" s="5" t="s">
@@ -716,7 +726,7 @@
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
-      <c r="D5" s="37"/>
+      <c r="D5" s="38"/>
     </row>
     <row r="6" spans="1:7" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
@@ -908,7 +918,9 @@
         <v>x0A</v>
       </c>
       <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
+      <c r="D18" s="34" t="s">
+        <v>8</v>
+      </c>
       <c r="E18" s="14"/>
       <c r="F18" s="28"/>
     </row>
@@ -922,7 +934,9 @@
         <v>x0B</v>
       </c>
       <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
+      <c r="D19" s="34" t="s">
+        <v>8</v>
+      </c>
       <c r="E19" s="14"/>
       <c r="F19" s="29"/>
     </row>
@@ -935,8 +949,12 @@
         <f t="shared" si="0"/>
         <v>x0C</v>
       </c>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14"/>
+      <c r="C20" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="D20" s="34" t="s">
+        <v>8</v>
+      </c>
       <c r="E20" s="14"/>
       <c r="F20" s="29"/>
     </row>
@@ -950,7 +968,9 @@
         <v>x0D</v>
       </c>
       <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
+      <c r="D21" s="34" t="s">
+        <v>8</v>
+      </c>
       <c r="E21" s="14"/>
       <c r="F21" s="29"/>
     </row>
@@ -964,7 +984,9 @@
         <v>x0E</v>
       </c>
       <c r="C22" s="14"/>
-      <c r="D22" s="14"/>
+      <c r="D22" s="34" t="s">
+        <v>8</v>
+      </c>
       <c r="E22" s="14"/>
       <c r="F22" s="29"/>
     </row>
@@ -978,7 +1000,9 @@
         <v>x0F</v>
       </c>
       <c r="C23" s="14"/>
-      <c r="D23" s="14"/>
+      <c r="D23" s="34" t="s">
+        <v>8</v>
+      </c>
       <c r="E23" s="14"/>
       <c r="F23" s="29"/>
     </row>
@@ -992,7 +1016,9 @@
         <v>x10</v>
       </c>
       <c r="C24" s="14"/>
-      <c r="D24" s="14"/>
+      <c r="D24" s="34" t="s">
+        <v>8</v>
+      </c>
       <c r="E24" s="14"/>
       <c r="F24" s="29"/>
     </row>
@@ -1006,7 +1032,9 @@
         <v>x11</v>
       </c>
       <c r="C25" s="14"/>
-      <c r="D25" s="14"/>
+      <c r="D25" s="34" t="s">
+        <v>8</v>
+      </c>
       <c r="E25" s="14"/>
       <c r="F25" s="29"/>
     </row>
@@ -1020,7 +1048,9 @@
         <v>x12</v>
       </c>
       <c r="C26" s="14"/>
-      <c r="D26" s="14"/>
+      <c r="D26" s="34" t="s">
+        <v>8</v>
+      </c>
       <c r="E26" s="14"/>
       <c r="F26" s="29"/>
     </row>
@@ -1034,7 +1064,9 @@
         <v>x13</v>
       </c>
       <c r="C27" s="14"/>
-      <c r="D27" s="14"/>
+      <c r="D27" s="34" t="s">
+        <v>8</v>
+      </c>
       <c r="E27" s="14"/>
       <c r="F27" s="29"/>
     </row>
@@ -1048,7 +1080,9 @@
         <v>x14</v>
       </c>
       <c r="C28" s="14"/>
-      <c r="D28" s="14"/>
+      <c r="D28" s="34" t="s">
+        <v>8</v>
+      </c>
       <c r="E28" s="14"/>
       <c r="F28" s="29"/>
     </row>
@@ -1062,7 +1096,9 @@
         <v>x15</v>
       </c>
       <c r="C29" s="14"/>
-      <c r="D29" s="14"/>
+      <c r="D29" s="34" t="s">
+        <v>8</v>
+      </c>
       <c r="E29" s="14"/>
       <c r="F29" s="29"/>
     </row>
@@ -1076,7 +1112,9 @@
         <v>x16</v>
       </c>
       <c r="C30" s="14"/>
-      <c r="D30" s="14"/>
+      <c r="D30" s="34" t="s">
+        <v>8</v>
+      </c>
       <c r="E30" s="14"/>
       <c r="F30" s="29"/>
     </row>
@@ -1090,7 +1128,9 @@
         <v>x17</v>
       </c>
       <c r="C31" s="14"/>
-      <c r="D31" s="14"/>
+      <c r="D31" s="34" t="s">
+        <v>8</v>
+      </c>
       <c r="E31" s="14"/>
       <c r="F31" s="29"/>
     </row>
@@ -1104,7 +1144,9 @@
         <v>x18</v>
       </c>
       <c r="C32" s="14"/>
-      <c r="D32" s="14"/>
+      <c r="D32" s="34" t="s">
+        <v>8</v>
+      </c>
       <c r="E32" s="14"/>
       <c r="F32" s="29"/>
     </row>
@@ -1118,7 +1160,9 @@
         <v>x19</v>
       </c>
       <c r="C33" s="14"/>
-      <c r="D33" s="14"/>
+      <c r="D33" s="34" t="s">
+        <v>8</v>
+      </c>
       <c r="E33" s="14"/>
       <c r="F33" s="29"/>
     </row>
@@ -1132,7 +1176,9 @@
         <v>x1A</v>
       </c>
       <c r="C34" s="14"/>
-      <c r="D34" s="14"/>
+      <c r="D34" s="34" t="s">
+        <v>8</v>
+      </c>
       <c r="E34" s="14"/>
       <c r="F34" s="29"/>
     </row>
@@ -1146,7 +1192,9 @@
         <v>x1B</v>
       </c>
       <c r="C35" s="14"/>
-      <c r="D35" s="14"/>
+      <c r="D35" s="34" t="s">
+        <v>8</v>
+      </c>
       <c r="E35" s="14"/>
       <c r="F35" s="29"/>
     </row>
@@ -1756,6 +1804,12 @@
       <c r="B85" s="19" t="str">
         <f t="shared" si="2"/>
         <v>x4D</v>
+      </c>
+      <c r="C85" t="s">
+        <v>74</v>
+      </c>
+      <c r="D85" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
add initial self-trigger handling
</commit_message>
<xml_diff>
--- a/doc/firmware-register-map-psec4a-evm.xlsx
+++ b/doc/firmware-register-map-psec4a-evm.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="80">
   <si>
     <t>Register Map</t>
   </si>
@@ -252,6 +252,18 @@
   </si>
   <si>
     <t>0=all samples, 1=ping-pong 528-sample blocks</t>
+  </si>
+  <si>
+    <t>psec4a self-trigger mode</t>
+  </si>
+  <si>
+    <t>00=off, 01=or trigger, 10=AND trigger, 11=sum trigger</t>
+  </si>
+  <si>
+    <t>psec4a self-trigger mask</t>
+  </si>
+  <si>
+    <t>lower 8 bits</t>
   </si>
 </sst>
 </file>
@@ -668,8 +680,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D91" sqref="D91"/>
+    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D79" sqref="D79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -677,7 +689,7 @@
     <col min="1" max="1" width="4.85546875" customWidth="1"/>
     <col min="2" max="2" width="8.42578125" style="13" customWidth="1"/>
     <col min="3" max="3" width="60.28515625" customWidth="1"/>
-    <col min="4" max="4" width="47.28515625" customWidth="1"/>
+    <col min="4" max="4" width="52.42578125" customWidth="1"/>
     <col min="5" max="5" width="12.7109375" customWidth="1"/>
     <col min="6" max="6" width="74.85546875" style="5" customWidth="1"/>
     <col min="7" max="7" width="7.42578125" customWidth="1"/>
@@ -1781,8 +1793,12 @@
         <f t="shared" si="2"/>
         <v>x4B</v>
       </c>
-      <c r="C83" s="8"/>
-      <c r="D83" s="17"/>
+      <c r="C83" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="D83" s="17" t="s">
+        <v>77</v>
+      </c>
       <c r="E83" s="8"/>
       <c r="F83" s="25"/>
     </row>
@@ -1794,6 +1810,12 @@
       <c r="B84" s="19" t="str">
         <f t="shared" si="2"/>
         <v>x4C</v>
+      </c>
+      <c r="C84" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="D84" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>